<commit_message>
Update Rizka - Cari Mobil Baru, Mobil Baru Kategori Daihatsu dan Toyota
</commit_message>
<xml_diff>
--- a/CariMobilBekasMarketplace.xlsx
+++ b/CariMobilBekasMarketplace.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORLD\KULIAH (TUGAS)\TGS SEMS. 8\INTERNSHIT\Task ACC ONE\ACC-ACCOne\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F35712CF-4822-4811-9178-76665B6043FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72FCD6E1-C6FA-45EF-B11F-390483F1EAD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7665" yWindow="795" windowWidth="13005" windowHeight="11070" xr2:uid="{3E3B5FBC-1010-4501-9539-40A745120687}"/>
+    <workbookView xWindow="7485" yWindow="0" windowWidth="13005" windowHeight="11070" activeTab="3" xr2:uid="{3E3B5FBC-1010-4501-9539-40A745120687}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Bekas" sheetId="1" r:id="rId1"/>
+    <sheet name="Baru" sheetId="2" r:id="rId2"/>
+    <sheet name="Daihatsu" sheetId="3" r:id="rId3"/>
+    <sheet name="Toyota" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="22">
   <si>
     <t>condition</t>
   </si>
@@ -54,6 +57,51 @@
   </si>
   <si>
     <t>failed</t>
+  </si>
+  <si>
+    <t>namaMobilBaru</t>
+  </si>
+  <si>
+    <t>Toyota Rush 2019</t>
+  </si>
+  <si>
+    <t>Daihatsu Sigra</t>
+  </si>
+  <si>
+    <t>Honda Brio</t>
+  </si>
+  <si>
+    <t>namaMobilDaihatsu</t>
+  </si>
+  <si>
+    <t>namaMobilToyota</t>
+  </si>
+  <si>
+    <t>Agya</t>
+  </si>
+  <si>
+    <t>Avanza</t>
+  </si>
+  <si>
+    <t>Rush</t>
+  </si>
+  <si>
+    <t>Yaris</t>
+  </si>
+  <si>
+    <t>Calya</t>
+  </si>
+  <si>
+    <t>Terios</t>
+  </si>
+  <si>
+    <t>Xenia</t>
+  </si>
+  <si>
+    <t>Ayla</t>
+  </si>
+  <si>
+    <t>Sigra</t>
   </si>
 </sst>
 </file>
@@ -70,15 +118,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -86,12 +146,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29216455-14D3-4160-A180-8013253E6754}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,34 +499,281 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C23F279B-AD0D-437C-9420-8E9090510E9C}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25E89210-B550-40EA-8A6A-892E2569B2D2}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEBEC4DA-F692-405D-8090-14CB87E90DA8}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Rizka - Update Data Binding Cari Mobil Baru 2
</commit_message>
<xml_diff>
--- a/CariMobilBekasMarketplace.xlsx
+++ b/CariMobilBekasMarketplace.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORLD\KULIAH (TUGAS)\TGS SEMS. 8\INTERNSHIT\Task ACC ONE\ACC-ACCOne\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72FCD6E1-C6FA-45EF-B11F-390483F1EAD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71FE4BB2-D502-49BF-BA98-99E18C4E35BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7485" yWindow="0" windowWidth="13005" windowHeight="11070" activeTab="3" xr2:uid="{3E3B5FBC-1010-4501-9539-40A745120687}"/>
+    <workbookView xWindow="7485" yWindow="0" windowWidth="13005" windowHeight="11070" activeTab="1" xr2:uid="{3E3B5FBC-1010-4501-9539-40A745120687}"/>
   </bookViews>
   <sheets>
     <sheet name="Bekas" sheetId="1" r:id="rId1"/>
@@ -62,9 +62,6 @@
     <t>namaMobilBaru</t>
   </si>
   <si>
-    <t>Toyota Rush 2019</t>
-  </si>
-  <si>
     <t>Daihatsu Sigra</t>
   </si>
   <si>
@@ -102,6 +99,9 @@
   </si>
   <si>
     <t>Sigra</t>
+  </si>
+  <si>
+    <t>Toyota Rush</t>
   </si>
 </sst>
 </file>
@@ -539,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C23F279B-AD0D-437C-9420-8E9090510E9C}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,7 +558,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
@@ -566,7 +566,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
@@ -574,7 +574,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>6</v>
@@ -601,7 +601,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -609,7 +609,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>6</v>
@@ -617,7 +617,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>6</v>
@@ -625,7 +625,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>6</v>
@@ -633,7 +633,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>6</v>
@@ -641,7 +641,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>6</v>
@@ -649,7 +649,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>5</v>
@@ -657,7 +657,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>5</v>
@@ -665,7 +665,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>5</v>
@@ -673,7 +673,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>5</v>
@@ -688,7 +688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEBEC4DA-F692-405D-8090-14CB87E90DA8}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -699,7 +699,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -707,7 +707,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>5</v>
@@ -715,7 +715,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>5</v>
@@ -723,7 +723,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>5</v>
@@ -731,7 +731,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>5</v>
@@ -739,7 +739,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>5</v>
@@ -747,7 +747,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>6</v>
@@ -755,7 +755,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>6</v>
@@ -763,7 +763,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>6</v>
@@ -771,7 +771,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Update Rizka - Data Ketinggalan
</commit_message>
<xml_diff>
--- a/CariMobilBekasMarketplace.xlsx
+++ b/CariMobilBekasMarketplace.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORLD\KULIAH (TUGAS)\TGS SEMS. 8\INTERNSHIT\Task ACC ONE\ACC-ACCOne\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71FE4BB2-D502-49BF-BA98-99E18C4E35BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C37D51-3671-4630-9CC2-4592428D318B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7485" yWindow="0" windowWidth="13005" windowHeight="11070" activeTab="1" xr2:uid="{3E3B5FBC-1010-4501-9539-40A745120687}"/>
+    <workbookView xWindow="885" yWindow="0" windowWidth="17895" windowHeight="11070" activeTab="1" xr2:uid="{3E3B5FBC-1010-4501-9539-40A745120687}"/>
   </bookViews>
   <sheets>
     <sheet name="Bekas" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="30">
   <si>
     <t>condition</t>
   </si>
@@ -62,12 +62,6 @@
     <t>namaMobilBaru</t>
   </si>
   <si>
-    <t>Daihatsu Sigra</t>
-  </si>
-  <si>
-    <t>Honda Brio</t>
-  </si>
-  <si>
     <t>namaMobilDaihatsu</t>
   </si>
   <si>
@@ -101,7 +95,37 @@
     <t>Sigra</t>
   </si>
   <si>
-    <t>Toyota Rush</t>
+    <t>paket</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Brio</t>
+  </si>
+  <si>
+    <t>spesific</t>
+  </si>
+  <si>
+    <t>Rush 1.5 G M/T</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>Rush 1.5 S TRD A/T</t>
+  </si>
+  <si>
+    <t>Sigra 1.2 R M/T DLX MC</t>
+  </si>
+  <si>
+    <t>Sigra 1.0 D M/T MC</t>
+  </si>
+  <si>
+    <t>Sigra 1.2 R A/T MC</t>
   </si>
 </sst>
 </file>
@@ -165,13 +189,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -537,48 +564,126 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C23F279B-AD0D-437C-9420-8E9090510E9C}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -601,7 +706,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -609,7 +714,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>6</v>
@@ -617,7 +722,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>6</v>
@@ -625,7 +730,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>6</v>
@@ -633,7 +738,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>6</v>
@@ -641,7 +746,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>6</v>
@@ -649,7 +754,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>5</v>
@@ -657,7 +762,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>5</v>
@@ -665,7 +770,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>5</v>
@@ -673,7 +778,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>5</v>
@@ -699,7 +804,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -707,7 +812,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>5</v>
@@ -715,7 +820,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>5</v>
@@ -723,7 +828,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>5</v>
@@ -731,7 +836,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>5</v>
@@ -739,7 +844,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>5</v>
@@ -747,7 +852,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>6</v>
@@ -755,7 +860,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>6</v>
@@ -763,7 +868,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>6</v>
@@ -771,7 +876,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Update Rizka - Edit Cari Promo + Tambah Data Binding
</commit_message>
<xml_diff>
--- a/CariMobilBekasMarketplace.xlsx
+++ b/CariMobilBekasMarketplace.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORLD\KULIAH (TUGAS)\TGS SEMS. 8\INTERNSHIT\Task ACC ONE\ACC-ACCOne\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C37D51-3671-4630-9CC2-4592428D318B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E17B7F6-C36E-4A83-8C24-A35CCD2C3849}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="885" yWindow="0" windowWidth="17895" windowHeight="11070" activeTab="1" xr2:uid="{3E3B5FBC-1010-4501-9539-40A745120687}"/>
   </bookViews>
@@ -567,7 +567,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update Rizka - Data tambahan
</commit_message>
<xml_diff>
--- a/CariMobilBekasMarketplace.xlsx
+++ b/CariMobilBekasMarketplace.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORLD\KULIAH (TUGAS)\TGS SEMS. 8\INTERNSHIT\Task ACC ONE\ACC-ACCOne\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E17B7F6-C36E-4A83-8C24-A35CCD2C3849}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B8AD51-AC19-4C63-951D-6A77AF79B9B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="885" yWindow="0" windowWidth="17895" windowHeight="11070" activeTab="1" xr2:uid="{3E3B5FBC-1010-4501-9539-40A745120687}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{3E3B5FBC-1010-4501-9539-40A745120687}"/>
   </bookViews>
   <sheets>
     <sheet name="Bekas" sheetId="1" r:id="rId1"/>
     <sheet name="Baru" sheetId="2" r:id="rId2"/>
-    <sheet name="Daihatsu" sheetId="3" r:id="rId3"/>
-    <sheet name="Toyota" sheetId="4" r:id="rId4"/>
+    <sheet name="BaruCampur" sheetId="6" r:id="rId3"/>
+    <sheet name="Daihatsu" sheetId="3" r:id="rId4"/>
+    <sheet name="Toyota" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="35">
   <si>
     <t>condition</t>
   </si>
@@ -126,19 +127,42 @@
   </si>
   <si>
     <t>Sigra 1.2 R A/T MC</t>
+  </si>
+  <si>
+    <t>biasa</t>
+  </si>
+  <si>
+    <t>daihatsuFailed</t>
+  </si>
+  <si>
+    <t>daihatsuPassed</t>
+  </si>
+  <si>
+    <t>toyotaPassed</t>
+  </si>
+  <si>
+    <t>toyotaFailed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -162,7 +186,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -185,11 +209,170 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -199,6 +382,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -566,15 +776,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C23F279B-AD0D-437C-9420-8E9090510E9C}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -691,11 +902,320 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71382B4D-F100-411A-B64E-E62F584953E2}">
+  <dimension ref="A1:D26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="25"/>
+      <c r="D8" s="27"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="14"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="14"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="14"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="14"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="14"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="12"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="12"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="12"/>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="29"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="9"/>
+      <c r="D18" s="10"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="12"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="12"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="12"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="12"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="14"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="4"/>
+      <c r="D24" s="14"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="4"/>
+      <c r="D25" s="14"/>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="16"/>
+      <c r="D26" s="17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25E89210-B550-40EA-8A6A-892E2569B2D2}">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -789,12 +1309,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEBEC4DA-F692-405D-8090-14CB87E90DA8}">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update Rizka - Fixing Data Binding
</commit_message>
<xml_diff>
--- a/CariMobilBekasMarketplace.xlsx
+++ b/CariMobilBekasMarketplace.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORLD\KULIAH (TUGAS)\TGS SEMS. 8\INTERNSHIT\Task ACC ONE\ACC-ACCOne\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520F9895-6B2D-46D8-A747-A246648596E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24EC8BAF-4652-484D-A7B9-8D61392A996A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{3E3B5FBC-1010-4501-9539-40A745120687}"/>
+    <workbookView xWindow="6105" yWindow="0" windowWidth="13440" windowHeight="11070" activeTab="2" xr2:uid="{3E3B5FBC-1010-4501-9539-40A745120687}"/>
   </bookViews>
   <sheets>
     <sheet name="Bekas" sheetId="1" r:id="rId1"/>
@@ -590,7 +590,7 @@
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -861,16 +861,16 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update Rizka - Update Object and Data Binding
</commit_message>
<xml_diff>
--- a/CariMobilBekasMarketplace.xlsx
+++ b/CariMobilBekasMarketplace.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORLD\KULIAH (TUGAS)\TGS SEMS. 8\INTERNSHIT\Task ACC ONE\ACC-ACCOne\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24EC8BAF-4652-484D-A7B9-8D61392A996A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3337D1-D499-492F-A20C-7AF8D66949F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6105" yWindow="0" windowWidth="13440" windowHeight="11070" activeTab="2" xr2:uid="{3E3B5FBC-1010-4501-9539-40A745120687}"/>
+    <workbookView xWindow="6450" yWindow="0" windowWidth="13440" windowHeight="11070" xr2:uid="{3E3B5FBC-1010-4501-9539-40A745120687}"/>
   </bookViews>
   <sheets>
     <sheet name="Bekas" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="43">
   <si>
     <t>condition</t>
   </si>
@@ -162,13 +162,10 @@
     <t>Toyota Calya 1.2 G M/T</t>
   </si>
   <si>
-    <t>New Ayla</t>
-  </si>
-  <si>
-    <t>Daihatsu Xenia 1.3 R CSTM A/T Bensin</t>
-  </si>
-  <si>
     <t>Daihatsu Ayla 1.2 R M/T</t>
+  </si>
+  <si>
+    <t>Daihatsu Xenia 1.3 R CSTM</t>
   </si>
 </sst>
 </file>
@@ -581,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29216455-14D3-4160-A180-8013253E6754}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,7 +629,7 @@
         <v>28</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="11" t="s">
@@ -660,10 +657,10 @@
         <v>28</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>36</v>
@@ -860,8 +857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71382B4D-F100-411A-B64E-E62F584953E2}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update Rizka - Test Case Logout
</commit_message>
<xml_diff>
--- a/CariMobilBekasMarketplace.xlsx
+++ b/CariMobilBekasMarketplace.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORLD\KULIAH (TUGAS)\TGS SEMS. 8\INTERNSHIT\Task ACC ONE\ACC-ACCOne\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3337D1-D499-492F-A20C-7AF8D66949F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF36E915-FCD6-44BA-AB73-8F983630A6D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6450" yWindow="0" windowWidth="13440" windowHeight="11070" xr2:uid="{3E3B5FBC-1010-4501-9539-40A745120687}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{3E3B5FBC-1010-4501-9539-40A745120687}"/>
   </bookViews>
   <sheets>
     <sheet name="Bekas" sheetId="1" r:id="rId1"/>
@@ -578,7 +578,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29216455-14D3-4160-A180-8013253E6754}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -857,8 +857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71382B4D-F100-411A-B64E-E62F584953E2}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Login, Cari mobil baru, mobil baru campur
</commit_message>
<xml_diff>
--- a/CariMobilBekasMarketplace.xlsx
+++ b/CariMobilBekasMarketplace.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORLD\KULIAH (TUGAS)\TGS SEMS. 8\INTERNSHIT\Task ACC ONE\ACC-ACCOne\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lieto\git\ACC-ACCOne\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF36E915-FCD6-44BA-AB73-8F983630A6D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{3E3B5FBC-1010-4501-9539-40A745120687}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Bekas" sheetId="1" r:id="rId1"/>
@@ -19,7 +18,7 @@
     <sheet name="Daihatsu" sheetId="3" r:id="rId4"/>
     <sheet name="Toyota" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="46">
   <si>
     <t>condition</t>
   </si>
@@ -108,18 +107,6 @@
     <t>all</t>
   </si>
   <si>
-    <t>Rush 1.5 S TRD A/T</t>
-  </si>
-  <si>
-    <t>Sigra 1.2 R M/T DLX MC</t>
-  </si>
-  <si>
-    <t>Sigra 1.0 D M/T MC</t>
-  </si>
-  <si>
-    <t>Sigra 1.2 R A/T MC</t>
-  </si>
-  <si>
     <t>daihatsuFailed</t>
   </si>
   <si>
@@ -166,12 +153,33 @@
   </si>
   <si>
     <t>Daihatsu Xenia 1.3 R CSTM</t>
+  </si>
+  <si>
+    <t>agya</t>
+  </si>
+  <si>
+    <t>Kijang</t>
+  </si>
+  <si>
+    <t>TOYOTA AGYA 1.0 G M/T NEW</t>
+  </si>
+  <si>
+    <t>TOYOTA AGYA 1.2 G M/T NEW</t>
+  </si>
+  <si>
+    <t>RUSH 1.5 G M/T</t>
+  </si>
+  <si>
+    <t>TOYOTA KIJANG INNOVA 2.0 Q M/T</t>
+  </si>
+  <si>
+    <t>DAIHATSU SIGRA 1.2 X M/T MC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -237,10 +245,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -262,6 +268,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -575,7 +582,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29216455-14D3-4160-A180-8013253E6754}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -592,131 +599,131 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="9" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
+      <c r="C2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="11" t="s">
+      <c r="B3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="D4" s="3"/>
+      <c r="E4" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="10" t="s">
-        <v>36</v>
+      <c r="B7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="8" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="10" t="s">
-        <v>37</v>
+      <c r="B8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="8" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="10"/>
+      <c r="B9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -725,18 +732,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C23F279B-AD0D-437C-9420-8E9090510E9C}">
-  <dimension ref="A1:D8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -747,106 +754,92 @@
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="B4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="2" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A7" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B7" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -854,10 +847,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71382B4D-F100-411A-B64E-E62F584953E2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -871,131 +864,131 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="9" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D4" s="3"/>
+      <c r="E4" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="10"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1003,7 +996,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25E89210-B550-40EA-8A6A-892E2569B2D2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1017,82 +1010,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1102,7 +1095,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEBEC4DA-F692-405D-8090-14CB87E90DA8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1115,82 +1108,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="3" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>